<commit_message>
se agrega test de formsPage
</commit_message>
<xml_diff>
--- a/dataset/demoQaExcel.xlsx
+++ b/dataset/demoQaExcel.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15270" windowHeight="4545" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15270" windowHeight="4545" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="textBox" sheetId="1" r:id="rId1"/>
     <sheet name="webTable" sheetId="2" r:id="rId2"/>
+    <sheet name="form" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>nombre</t>
   </si>
@@ -97,6 +98,30 @@
   </si>
   <si>
     <t>QA testing</t>
+  </si>
+  <si>
+    <t>celu</t>
+  </si>
+  <si>
+    <t>direccion</t>
+  </si>
+  <si>
+    <t>montNumber</t>
+  </si>
+  <si>
+    <t>año</t>
+  </si>
+  <si>
+    <t>materia</t>
+  </si>
+  <si>
+    <t>rodri@gmial.com</t>
+  </si>
+  <si>
+    <t>gil barros</t>
+  </si>
+  <si>
+    <t>english</t>
   </si>
 </sst>
 </file>
@@ -509,7 +534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -567,4 +592,78 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2">
+        <v>1234567890</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2">
+        <v>11</v>
+      </c>
+      <c r="G2">
+        <v>1988</v>
+      </c>
+      <c r="H2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>